<commit_message>
our final, jhyau for juniors
</commit_message>
<xml_diff>
--- a/Documents/Final/candidates-final.xlsx
+++ b/Documents/Final/candidates-final.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Roll NO</t>
   </si>
@@ -30,21 +30,6 @@
   </si>
   <si>
     <t xml:space="preserve"> External Examiner</t>
-  </si>
-  <si>
-    <t>077bct098</t>
-  </si>
-  <si>
-    <t>darpan</t>
-  </si>
-  <si>
-    <t>hehe</t>
-  </si>
-  <si>
-    <t>Dr. Darpan  Kattel</t>
-  </si>
-  <si>
-    <t>Mr. Saurav  Dhungana</t>
   </si>
 </sst>
 </file>
@@ -393,7 +378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,23 +403,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>